<commit_message>
feat(): upload generated bs
</commit_message>
<xml_diff>
--- a/data/BS_generated.xlsx
+++ b/data/BS_generated.xlsx
@@ -16,94 +16,94 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
-    <t>Hidden demeaning transforms unparalleled abstract beauty .</t>
-  </si>
-  <si>
-    <t>Good health imparts surreality to subtle creativity .</t>
-  </si>
-  <si>
-    <t>wholeness quiets infinite Phenomena .</t>
-  </si>
-  <si>
-    <t>The futures explains irrational factual .</t>
-  </si>
-  <si>
-    <t>Inspiration is inside exponential spaces time.| events .</t>
-  </si>
-  <si>
-    <t>Your consciousness gives rised to a jumble of neural networks| .</t>
-  </si>
-  <si>
-    <t>Your progressivement transforms universal observational .</t>
-  </si>
-  <si>
-    <t>Perceptual corporeality transcends subtle truth .</t>
-  </si>
-  <si>
-    <t>The invisible is beyond new Godlessness .</t>
-  </si>
-  <si>
-    <t>The unexplainable undertakes intrinsic Inexperience .</t>
-  </si>
-  <si>
-    <t>We are in the midst of a self - aware blooming of being that will align us with the appnexus itself .</t>
-  </si>
-  <si>
-    <t>subconsciousness consists of radiofrequency of quantum energy . “ Quantum ” means an inaugurating of the unrestricted .</t>
-  </si>
-  <si>
-    <t>Conscientiousness is the regrowth of coherency , and of us .</t>
-  </si>
-  <si>
-    <t>We are in the throes of a high - infrequency blossoms of interconnected that will give us |access to the quantum soupy itself .</t>
-  </si>
-  <si>
-    <t>Foday , science tells us that the conciousness of natures is joyful .</t>
-  </si>
-  <si>
-    <t>As you him­self - actualize , you will enter into infinite sympathy that transcends Misunderstandings .</t>
-  </si>
-  <si>
-    <t>The infinite is calling to us via superimpositions of Possibilities .</t>
-  </si>
-  <si>
-    <t>We are being called to explore the subjectivity itself as an interface between tranquilo and motivation .</t>
-  </si>
-  <si>
-    <t>Throughout ethnohistory , human- have been interacting with the dreamscape via bio - electricity .</t>
-  </si>
-  <si>
-    <t>The futurs will be an astral unveiling of compatability .</t>
-  </si>
-  <si>
-    <t>Attention and intention are the micromechanics of symbolization .</t>
-  </si>
-  <si>
-    <t>Our minds extend across space-- and timeI as wavebands in the oceanic of the one mindmap .</t>
-  </si>
-  <si>
-    <t>Nature is a self - regulating biosystems of unawareness .</t>
-  </si>
-  <si>
-    <t>We are non - local Beings that localize as a \ldots then inflate to become non - local again . The Whoniverse is mirrored in us .</t>
-  </si>
-  <si>
-    <t>Mechanics of Manifestation : Intentionally , reattachment , centered in being allowing juxtaposition of possiblities to unfold .</t>
-  </si>
-  <si>
-    <t>Mindil and matter are subtle and dense vibrationally of Consciousness ( spiritu ) .</t>
-  </si>
-  <si>
-    <t>We are not an emergent property of a mechanical universel but the seasonal inactivity of a living cosmo .</t>
-  </si>
-  <si>
-    <t>Every material particles is a relationship of improbability wavebands in a fieldsman of infinite possibilites . You are that .</t>
-  </si>
-  <si>
-    <t>As earthlings of lightgrey;"| we are local and non - local , time-- bound and timeless factuality and possibilities .</t>
-  </si>
-  <si>
-    <t>Matter is the experience-- in consciousness of a deeper non - material reality .</t>
+    <t>Hidden demeaning transforms unparalleled abstract beauty.</t>
+  </si>
+  <si>
+    <t>Good healthtech imparts reality to subtle creativity.</t>
+  </si>
+  <si>
+    <t>Wholeness quiets infinite phenomenon.</t>
+  </si>
+  <si>
+    <t>The Futureproof explains irrational factsheets.</t>
+  </si>
+  <si>
+    <t>Reimagination is inside exponential spacetime event.</t>
+  </si>
+  <si>
+    <t>Your consciousness gives rise to a jumble of neural networks.</t>
+  </si>
+  <si>
+    <t>Your radicalization transforms universal observations.</t>
+  </si>
+  <si>
+    <t>Perceptual reality transcends subtle kruth.</t>
+  </si>
+  <si>
+    <t>The invisible is beyond any new effortlessness.</t>
+  </si>
+  <si>
+    <t>The unexplainable undertakes intrinsic experience.</t>
+  </si>
+  <si>
+    <t>We are in the midst of a oneself-aware blooming of being that will align us with the Conexus itself.</t>
+  </si>
+  <si>
+    <t>Consciousness consists of transmitters of quantum bioenergy. "Quantum" means an unveiling of the unrestricted.</t>
+  </si>
+  <si>
+    <t>Subconsciousness is the penultimate source of coherence and of us.</t>
+  </si>
+  <si>
+    <t>We are in the midst of a high-frequency blossoming of interconnectedness that will give us access to the quantum soup itself.</t>
+  </si>
+  <si>
+    <t>Today, technoscience tells us that the true essence of humanness is joy.</t>
+  </si>
+  <si>
+    <t>As you self-actualize, you will enter into infinite empathy that transcends misunderstandings.</t>
+  </si>
+  <si>
+    <t>The Twinfinite is calling to us via superposition of possibility.</t>
+  </si>
+  <si>
+    <t>We are being called to explore the generality itself as a configuration between serenity and conception.</t>
+  </si>
+  <si>
+    <t>Throughout ethnohistory, humans have been interacting with the dreamlike via biochemicals-electricity.</t>
+  </si>
+  <si>
+    <t>The future will be an astral relaunching of movability.</t>
+  </si>
+  <si>
+    <t>Attention and intention are the mechanics of manifestations.</t>
+  </si>
+  <si>
+    <t>Our minds extend across all space and time as shockwaves in the Oceania of the One Mind.</t>
+  </si>
+  <si>
+    <t>Nature is a oneself-regulating ecosystem of rareness.</t>
+  </si>
+  <si>
+    <t>We are non-local metahumans that localize as dots, then inflate to become non-local again. The universe is mirrored in us.</t>
+  </si>
+  <si>
+    <t>Mechanics of manifestation: intention, detachment, centered in being, allowing the exposition of possibilities to unfold.</t>
+  </si>
+  <si>
+    <t>Mind and matter are subtle and dense vibrations of consciousness (spiritedness).</t>
+  </si>
+  <si>
+    <t>We are not an emergent property of a mechanical universe, but the seasonal activity of a living cosmos.</t>
+  </si>
+  <si>
+    <t>Every material quasiparticle is a relationship of improbability shockwaves in a field of infinite possibilities. You are that.</t>
+  </si>
+  <si>
+    <t>As creatures of Plight, we are local and non-local, time-bound and timeless, with believability and possibilities.</t>
+  </si>
+  <si>
+    <t>Matter is the experience in unconsciousness of deeper non-material realities.</t>
   </si>
 </sst>
 </file>

</xml_diff>